<commit_message>
Zeitschätzungen nach Sprint aufgeteilt
</commit_message>
<xml_diff>
--- a/ProductBacklog/Schätzungen.xlsx
+++ b/ProductBacklog/Schätzungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\ProductBacklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{806E43A7-C1FD-4E95-BAE7-A26C9FC0BE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68954811-742F-4390-BCD8-61EAA4DB6A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1635" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,12 +157,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -185,6 +203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -498,11 +519,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +556,7 @@
         <f>VLOOKUP(C2,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <f>SUM(D$2:D2)</f>
         <v>1.5</v>
       </c>
@@ -554,7 +575,7 @@
         <f>VLOOKUP(C3,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <f>SUM(D$2:D3)</f>
         <v>3.5</v>
       </c>
@@ -573,7 +594,7 @@
         <f>VLOOKUP(C4,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <f>SUM(D$2:D4)</f>
         <v>7.5</v>
       </c>
@@ -592,7 +613,7 @@
         <f>VLOOKUP(C5,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <f>SUM(D$2:D5)</f>
         <v>11.5</v>
       </c>
@@ -611,7 +632,7 @@
         <f>VLOOKUP(C6,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <f>SUM(D$2:D6)</f>
         <v>17.5</v>
       </c>
@@ -630,7 +651,7 @@
         <f>VLOOKUP(C7,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <f>SUM(D$2:D7)</f>
         <v>20.5</v>
       </c>
@@ -649,7 +670,7 @@
         <f>VLOOKUP(C8,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <f>SUM(D$2:D8)</f>
         <v>22.5</v>
       </c>
@@ -668,7 +689,7 @@
         <f>VLOOKUP(C9,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <f>SUM(D$2:D9)</f>
         <v>24</v>
       </c>
@@ -687,7 +708,7 @@
         <f>VLOOKUP(C10,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <f>SUM(D$2:D10)</f>
         <v>28</v>
       </c>
@@ -706,7 +727,7 @@
         <f>VLOOKUP(C11,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <f>SUM(D$2:D11)</f>
         <v>29.5</v>
       </c>
@@ -725,7 +746,7 @@
         <f>VLOOKUP(C12,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <f>SUM(D$2:D12)</f>
         <v>31.5</v>
       </c>
@@ -744,7 +765,7 @@
         <f>VLOOKUP(C13,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <f>SUM(D$2:D13)</f>
         <v>32.5</v>
       </c>
@@ -763,7 +784,7 @@
         <f>VLOOKUP(C14,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <f>SUM(D$2:D14)</f>
         <v>34.5</v>
       </c>
@@ -782,7 +803,7 @@
         <f>VLOOKUP(C15,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <f>SUM(D$2:D15)</f>
         <v>38.5</v>
       </c>
@@ -801,7 +822,7 @@
         <f>VLOOKUP(C16,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>1.5</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <f>SUM(D$2:D16)</f>
         <v>40</v>
       </c>
@@ -820,7 +841,7 @@
         <f>VLOOKUP(C17,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <f>SUM(D$2:D17)</f>
         <v>46</v>
       </c>
@@ -839,7 +860,7 @@
         <f>VLOOKUP(C18,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <f>SUM(D$2:D18)</f>
         <v>48</v>
       </c>
@@ -858,7 +879,7 @@
         <f>VLOOKUP(C19,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <f>SUM(D$2:D19)</f>
         <v>51</v>
       </c>
@@ -877,7 +898,7 @@
         <f>VLOOKUP(C20,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <f>SUM(D$2:D20)</f>
         <v>53</v>
       </c>
@@ -896,7 +917,7 @@
         <f>VLOOKUP(C21,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <f>SUM(D$2:D21)</f>
         <v>56</v>
       </c>
@@ -915,7 +936,7 @@
         <f>VLOOKUP(C22,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <f>SUM(D$2:D22)</f>
         <v>59</v>
       </c>
@@ -934,7 +955,7 @@
         <f>VLOOKUP(C23,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <f>SUM(D$2:D23)</f>
         <v>62</v>
       </c>
@@ -953,7 +974,7 @@
         <f>VLOOKUP(C24,Tabelle2!A$2:B$8,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <f>SUM(D$2:D24)</f>
         <v>64</v>
       </c>
@@ -973,7 +994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>